<commit_message>
Add enlace Jira + act itinerario
</commit_message>
<xml_diff>
--- a/Cronograma/ActividadesPracticas_Rodriguez.V1.1 .xlsx
+++ b/Cronograma/ActividadesPracticas_Rodriguez.V1.1 .xlsx
@@ -13,8 +13,36 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="C36">
+      <text>
+        <t xml:space="preserve">table
+	-Betty Rodriguez</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C47">
+      <text>
+        <t xml:space="preserve">generate pdf
+	-Betty Rodriguez</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C50">
+      <text>
+        <t xml:space="preserve">swagger
+	-Betty Rodriguez</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="114">
   <si>
     <t>ACTIVIDADES REALIZADAS EN LA UNIDAD DE DESARROLLO INFORMATICO</t>
   </si>
@@ -85,10 +113,7 @@
     <t>Implementación de elementos interactivos en la interfaz</t>
   </si>
   <si>
-    <t>Codificación de funcionalidades para la sección "Ver Resultado"</t>
-  </si>
-  <si>
-    <t>Codificación de funcionalidades para la seccion "Ver Resultado"</t>
+    <t>Implementación de funcionalidades para la sección "Ver Auditorias" en la carpeta de desarrollo de componentes Services, controller, Rutes.</t>
   </si>
   <si>
     <t>Desarrollo de funcionalidades para las secciones "Filtrar Auditorías" y Incorporación de la función de exportación de auditorías,Conexión entre la interfaz de usuario y los servicios del backend</t>
@@ -133,10 +158,10 @@
     <t>NUMERO DE HORAS</t>
   </si>
   <si>
-    <t>Presentación e indución de lineamientos</t>
-  </si>
-  <si>
-    <t>Inducción y presentación sobre la infrestructura en la Fundación con Cristo</t>
+    <t>Presentación e inducción de lineamientos</t>
+  </si>
+  <si>
+    <t>Inducción y presentación sobre la infraestructura en la Fundación con Cristo</t>
   </si>
   <si>
     <t>09:00 -12:00</t>
@@ -205,12 +230,12 @@
     <t>Configurar las relaciones con tabla de usuario y módulos del sistema</t>
   </si>
   <si>
+    <t>Elaborar Diagrama de la base de datos para auditorías.</t>
+  </si>
+  <si>
     <t>Diseño el módulo auditorías</t>
   </si>
   <si>
-    <t>Elaborar Diagrama de la base de datos para auditorías.</t>
-  </si>
-  <si>
     <t>Elaborar Flujo de navegación entre las  secciones "Ver auditorías", "Filtrar Auditoria",Exportar Auditorías" del módulo.</t>
   </si>
   <si>
@@ -241,18 +266,9 @@
     <t>Implementar botones funcionales: "Ver Historial", "Filtrar", y "Exportar".</t>
   </si>
   <si>
-    <t>Implementación de funcionalidades para la sección "Ver Auditoriìas"</t>
-  </si>
-  <si>
     <t>Desarrollar la capacidad y funcionalidad de obtener y mostrar el listado completo de auditorías.</t>
   </si>
   <si>
-    <t>Implementación de funcionalidades para la sección "Ver Auditorìas"</t>
-  </si>
-  <si>
-    <t>Desarrollar la funcionalidad para recuperar el listado completo de auditorías</t>
-  </si>
-  <si>
     <t>Implementar opciones de filtrado (usuario, fecha) en el sistema de auditorías para obtener resultados específicos.</t>
   </si>
   <si>
@@ -283,7 +299,7 @@
     <t>Elaborar una guía de usuario detallada sobre la navegación y uso de las funciones de auditoría.</t>
   </si>
   <si>
-    <t>Publicar la aplicación en componentes servidor cliente</t>
+    <t>Subir el proyecto modificado al respositorio FTP de la fundación</t>
   </si>
   <si>
     <t>Capacitar a los usuarios clave.</t>
@@ -368,12 +384,6 @@
   </si>
   <si>
     <t>HORA TRABAJADA POR DÍA</t>
-  </si>
-  <si>
-    <t>Feriado</t>
-  </si>
-  <si>
-    <t>Feriado segun calendario académico</t>
   </si>
 </sst>
 </file>
@@ -852,7 +862,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="104">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1054,9 +1064,6 @@
     <xf borderId="2" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="5" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -1139,9 +1146,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="46" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1374,7 +1378,6 @@
     <col customWidth="1" min="1" max="1" width="17.25"/>
     <col customWidth="1" min="2" max="2" width="66.13"/>
     <col customWidth="1" hidden="1" min="3" max="3" width="16.75"/>
-    <col customWidth="1" min="5" max="5" width="12.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1625,7 +1628,7 @@
       <c r="A32" s="13">
         <v>45646.0</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="16"/>
@@ -1634,9 +1637,7 @@
       <c r="A33" s="13">
         <v>45663.0</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>24</v>
-      </c>
+      <c r="B33" s="15"/>
       <c r="C33" s="18"/>
     </row>
     <row r="34">
@@ -1672,7 +1673,7 @@
         <v>45670.0</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C38" s="18"/>
     </row>
@@ -1744,7 +1745,7 @@
         <v>45684.0</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C48" s="18"/>
     </row>
@@ -1760,7 +1761,7 @@
         <v>45686.0</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C50" s="15"/>
     </row>
@@ -1788,26 +1789,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B27:B31"/>
     <mergeCell ref="C33:C37"/>
     <mergeCell ref="C38:C42"/>
+    <mergeCell ref="B38:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="B32:B37"/>
     <mergeCell ref="C43:C47"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B38:B47"/>
-    <mergeCell ref="B33:B37"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B19"/>
     <mergeCell ref="C14:C18"/>
     <mergeCell ref="C19:C22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1833,12 +1834,12 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="23">
         <v>45614.0</v>
@@ -1846,7 +1847,7 @@
     </row>
     <row r="3">
       <c r="A3" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="24">
         <v>45687.0</v>
@@ -1854,7 +1855,7 @@
     </row>
     <row r="4">
       <c r="A4" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>6</v>
@@ -1862,7 +1863,7 @@
     </row>
     <row r="5">
       <c r="A5" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>8</v>
@@ -1870,7 +1871,7 @@
     </row>
     <row r="6">
       <c r="A6" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>10</v>
@@ -1881,20 +1882,20 @@
         <v>11</v>
       </c>
       <c r="B8" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="D8" s="27" t="s">
         <v>35</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>36</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="27" t="s">
         <v>37</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9">
@@ -1902,19 +1903,19 @@
         <v>45614.0</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="D9" s="30" t="s">
         <v>40</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>41</v>
       </c>
       <c r="E9" s="30">
         <v>3.0</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="32">
         <f>E9+E10</f>
@@ -1926,10 +1927,10 @@
       <c r="A10" s="34"/>
       <c r="B10" s="19"/>
       <c r="C10" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="36" t="s">
         <v>43</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>44</v>
       </c>
       <c r="E10" s="36">
         <v>3.0</v>
@@ -1942,19 +1943,19 @@
         <v>45615.0</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="D11" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="E11" s="30">
+        <v>6.0</v>
+      </c>
+      <c r="F11" s="31" t="s">
         <v>47</v>
-      </c>
-      <c r="E11" s="30">
-        <v>6.0</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>48</v>
       </c>
       <c r="G11" s="40">
         <v>6.0</v>
@@ -1967,10 +1968,10 @@
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="43">
         <v>6.0</v>
@@ -1987,10 +1988,10 @@
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="43">
         <v>6.0</v>
@@ -2007,10 +2008,10 @@
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="43">
         <v>3.0</v>
@@ -2025,10 +2026,10 @@
       <c r="A15" s="34"/>
       <c r="B15" s="19"/>
       <c r="C15" s="49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="36">
         <v>3.0</v>
@@ -2045,16 +2046,16 @@
         <v>17</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="30">
+        <v>6.0</v>
+      </c>
+      <c r="F16" s="31" t="s">
         <v>47</v>
-      </c>
-      <c r="E16" s="30">
-        <v>6.0</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>48</v>
       </c>
       <c r="G16" s="40">
         <v>6.0</v>
@@ -2067,10 +2068,10 @@
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="43">
         <v>6.0</v>
@@ -2087,10 +2088,10 @@
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="43">
         <v>6.0</v>
@@ -2108,10 +2109,10 @@
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="43">
         <v>6.0</v>
@@ -2128,10 +2129,10 @@
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="43">
         <v>6.0</v>
@@ -2148,10 +2149,10 @@
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="36">
         <v>6.0</v>
@@ -2166,19 +2167,19 @@
         <v>45629.0</v>
       </c>
       <c r="B22" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="56" t="s">
-        <v>60</v>
-      </c>
       <c r="D22" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="57">
+        <v>6.0</v>
+      </c>
+      <c r="F22" s="58" t="s">
         <v>47</v>
-      </c>
-      <c r="E22" s="57">
-        <v>6.0</v>
-      </c>
-      <c r="F22" s="58" t="s">
-        <v>48</v>
       </c>
       <c r="G22" s="59">
         <v>6.0</v>
@@ -2192,16 +2193,16 @@
         <v>19</v>
       </c>
       <c r="C23" s="60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="30">
+        <v>6.0</v>
+      </c>
+      <c r="F23" s="31" t="s">
         <v>47</v>
-      </c>
-      <c r="E23" s="30">
-        <v>6.0</v>
-      </c>
-      <c r="F23" s="31" t="s">
-        <v>48</v>
       </c>
       <c r="G23" s="40">
         <v>6.0</v>
@@ -2211,12 +2212,12 @@
       <c r="A24" s="51">
         <v>45631.0</v>
       </c>
-      <c r="B24" s="19"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="36">
         <v>6.0</v>
@@ -2230,20 +2231,18 @@
       <c r="A25" s="38">
         <v>45635.0</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>63</v>
-      </c>
+      <c r="B25" s="19"/>
       <c r="C25" s="62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D25" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="30">
+        <v>6.0</v>
+      </c>
+      <c r="F25" s="31" t="s">
         <v>47</v>
-      </c>
-      <c r="E25" s="30">
-        <v>6.0</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>48</v>
       </c>
       <c r="G25" s="40">
         <v>6.0</v>
@@ -2253,12 +2252,14 @@
       <c r="A26" s="41">
         <v>45636.0</v>
       </c>
-      <c r="B26" s="15"/>
+      <c r="B26" s="17" t="s">
+        <v>63</v>
+      </c>
       <c r="C26" s="63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="43">
         <v>6.0</v>
@@ -2274,10 +2275,10 @@
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" s="36">
         <v>6.0</v>
@@ -2295,16 +2296,16 @@
         <v>21</v>
       </c>
       <c r="C28" s="65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" s="43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28" s="66">
         <v>3.0</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G28" s="67">
         <f>E28+E29+E30</f>
@@ -2315,10 +2316,10 @@
       <c r="A29" s="68"/>
       <c r="B29" s="15"/>
       <c r="C29" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="66" t="s">
         <v>69</v>
-      </c>
-      <c r="D29" s="66" t="s">
-        <v>70</v>
       </c>
       <c r="E29" s="66">
         <v>2.0</v>
@@ -2330,10 +2331,10 @@
       <c r="A30" s="34"/>
       <c r="B30" s="19"/>
       <c r="C30" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="36" t="s">
         <v>71</v>
-      </c>
-      <c r="D30" s="36" t="s">
-        <v>72</v>
       </c>
       <c r="E30" s="70">
         <v>1.0</v>
@@ -2349,16 +2350,16 @@
         <v>22</v>
       </c>
       <c r="C31" s="71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D31" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="30">
+        <v>6.0</v>
+      </c>
+      <c r="F31" s="31" t="s">
         <v>47</v>
-      </c>
-      <c r="E31" s="30">
-        <v>6.0</v>
-      </c>
-      <c r="F31" s="31" t="s">
-        <v>48</v>
       </c>
       <c r="G31" s="40">
         <v>6.0</v>
@@ -2371,7 +2372,7 @@
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
       <c r="D32" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E32" s="43">
         <v>6.0</v>
@@ -2387,10 +2388,10 @@
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D33" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E33" s="43">
         <v>6.0</v>
@@ -2407,7 +2408,7 @@
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E34" s="43">
         <v>6.0</v>
@@ -2424,7 +2425,7 @@
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
       <c r="D35" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E35" s="36">
         <v>6.0</v>
@@ -2438,20 +2439,20 @@
       <c r="A36" s="54">
         <v>45646.0</v>
       </c>
-      <c r="B36" s="55" t="s">
-        <v>75</v>
+      <c r="B36" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="C36" s="73" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D36" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="57">
+        <v>6.0</v>
+      </c>
+      <c r="F36" s="58" t="s">
         <v>47</v>
-      </c>
-      <c r="E36" s="57">
-        <v>6.0</v>
-      </c>
-      <c r="F36" s="58" t="s">
-        <v>48</v>
       </c>
       <c r="G36" s="59">
         <v>6.0</v>
@@ -2461,20 +2462,16 @@
       <c r="A37" s="38">
         <v>45663.0</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="74" t="s">
-        <v>78</v>
-      </c>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="30">
+        <v>6.0</v>
+      </c>
+      <c r="F37" s="31" t="s">
         <v>47</v>
-      </c>
-      <c r="E37" s="30">
-        <v>6.0</v>
-      </c>
-      <c r="F37" s="31" t="s">
-        <v>48</v>
       </c>
       <c r="G37" s="40">
         <v>6.0</v>
@@ -2487,7 +2484,7 @@
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E38" s="43">
         <v>6.0</v>
@@ -2504,7 +2501,7 @@
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E39" s="43">
         <v>6.0</v>
@@ -2521,7 +2518,7 @@
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E40" s="43">
         <v>6.0</v>
@@ -2538,7 +2535,7 @@
       <c r="B41" s="19"/>
       <c r="C41" s="19"/>
       <c r="D41" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E41" s="36">
         <v>6.0</v>
@@ -2553,19 +2550,19 @@
         <v>45670.0</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="74" t="s">
-        <v>79</v>
+        <v>24</v>
+      </c>
+      <c r="C42" s="73" t="s">
+        <v>75</v>
       </c>
       <c r="D42" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="30">
+        <v>6.0</v>
+      </c>
+      <c r="F42" s="31" t="s">
         <v>47</v>
-      </c>
-      <c r="E42" s="30">
-        <v>6.0</v>
-      </c>
-      <c r="F42" s="31" t="s">
-        <v>48</v>
       </c>
       <c r="G42" s="40">
         <v>6.0</v>
@@ -2578,7 +2575,7 @@
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E43" s="43">
         <v>6.0</v>
@@ -2595,7 +2592,7 @@
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E44" s="43">
         <v>6.0</v>
@@ -2612,7 +2609,7 @@
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
       <c r="D45" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E45" s="43">
         <v>6.0</v>
@@ -2629,7 +2626,7 @@
       <c r="B46" s="15"/>
       <c r="C46" s="16"/>
       <c r="D46" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E46" s="43">
         <v>6.0</v>
@@ -2644,11 +2641,11 @@
         <v>45677.0</v>
       </c>
       <c r="B47" s="15"/>
-      <c r="C47" s="75" t="s">
-        <v>80</v>
+      <c r="C47" s="74" t="s">
+        <v>76</v>
       </c>
       <c r="D47" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E47" s="43">
         <v>6.0</v>
@@ -2665,7 +2662,7 @@
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
       <c r="D48" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E48" s="43">
         <v>6.0</v>
@@ -2682,7 +2679,7 @@
       <c r="B49" s="15"/>
       <c r="C49" s="16"/>
       <c r="D49" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E49" s="43">
         <v>6.0</v>
@@ -2697,17 +2694,17 @@
         <v>45680.0</v>
       </c>
       <c r="B50" s="15"/>
-      <c r="C50" s="76" t="s">
-        <v>81</v>
+      <c r="C50" s="75" t="s">
+        <v>77</v>
       </c>
       <c r="D50" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" s="43">
+        <v>6.0</v>
+      </c>
+      <c r="F50" s="76" t="s">
         <v>47</v>
-      </c>
-      <c r="E50" s="43">
-        <v>6.0</v>
-      </c>
-      <c r="F50" s="77" t="s">
-        <v>48</v>
       </c>
       <c r="G50" s="44">
         <v>6.0</v>
@@ -2720,7 +2717,7 @@
       <c r="B51" s="19"/>
       <c r="C51" s="19"/>
       <c r="D51" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E51" s="36">
         <v>6.0</v>
@@ -2735,49 +2732,49 @@
         <v>45684.0</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C52" s="78" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="C52" s="77" t="s">
+        <v>79</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E52" s="30">
         <v>3.0</v>
       </c>
       <c r="F52" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G52" s="32">
         <v>6.0</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="79"/>
+      <c r="A53" s="78"/>
       <c r="B53" s="15"/>
-      <c r="C53" s="80" t="s">
-        <v>84</v>
+      <c r="C53" s="79" t="s">
+        <v>80</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E53" s="43">
         <v>3.0</v>
       </c>
       <c r="F53" s="15"/>
-      <c r="G53" s="81"/>
+      <c r="G53" s="80"/>
     </row>
     <row r="54">
       <c r="A54" s="46">
         <v>45685.0</v>
       </c>
       <c r="B54" s="15"/>
-      <c r="C54" s="80" t="s">
-        <v>85</v>
+      <c r="C54" s="79" t="s">
+        <v>81</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E54" s="43">
         <v>3.0</v>
@@ -2790,11 +2787,11 @@
     <row r="55">
       <c r="A55" s="34"/>
       <c r="B55" s="19"/>
-      <c r="C55" s="82" t="s">
-        <v>86</v>
+      <c r="C55" s="81" t="s">
+        <v>82</v>
       </c>
       <c r="D55" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E55" s="36">
         <v>3.0</v>
@@ -2807,19 +2804,19 @@
         <v>45686.0</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C56" s="83" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="C56" s="82" t="s">
+        <v>84</v>
       </c>
       <c r="D56" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" s="30">
+        <v>6.0</v>
+      </c>
+      <c r="F56" s="31" t="s">
         <v>47</v>
-      </c>
-      <c r="E56" s="30">
-        <v>6.0</v>
-      </c>
-      <c r="F56" s="31" t="s">
-        <v>48</v>
       </c>
       <c r="G56" s="40">
         <v>6.0</v>
@@ -2830,11 +2827,11 @@
         <v>45687.0</v>
       </c>
       <c r="B57" s="15"/>
-      <c r="C57" s="84" t="s">
-        <v>89</v>
+      <c r="C57" s="83" t="s">
+        <v>85</v>
       </c>
       <c r="D57" s="66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E57" s="43">
         <v>3.0</v>
@@ -2847,11 +2844,11 @@
     <row r="58">
       <c r="A58" s="34"/>
       <c r="B58" s="19"/>
-      <c r="C58" s="85" t="s">
-        <v>90</v>
+      <c r="C58" s="84" t="s">
+        <v>86</v>
       </c>
       <c r="D58" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E58" s="36">
         <v>3.0</v>
@@ -2861,26 +2858,26 @@
     </row>
     <row r="59">
       <c r="A59" s="20"/>
-      <c r="D59" s="86" t="s">
-        <v>91</v>
-      </c>
-      <c r="E59" s="87">
+      <c r="D59" s="85" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" s="86">
         <f>SUM(E9:E36,E37:E58)</f>
         <v>258</v>
       </c>
-      <c r="F59" s="88" t="s">
-        <v>91</v>
-      </c>
-      <c r="G59" s="86">
+      <c r="F59" s="87" t="s">
+        <v>87</v>
+      </c>
+      <c r="G59" s="85">
         <f>SUM(G9:G58)</f>
         <v>258</v>
       </c>
     </row>
     <row r="60">
-      <c r="G60" s="89"/>
+      <c r="G60" s="88"/>
     </row>
     <row r="61">
-      <c r="G61" s="89"/>
+      <c r="G61" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -2901,8 +2898,8 @@
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B16:B21"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B27"/>
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="F42:F49"/>
@@ -2916,23 +2913,24 @@
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="F31:F35"/>
     <mergeCell ref="C33:C35"/>
-    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="C36:C41"/>
     <mergeCell ref="F37:F41"/>
     <mergeCell ref="C47:C49"/>
     <mergeCell ref="B56:B58"/>
     <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="B42:B51"/>
     <mergeCell ref="C42:C46"/>
+    <mergeCell ref="C50:C51"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="A54:A55"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="B42:B51"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2954,15 +2952,15 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="23">
         <v>45614.0</v>
@@ -2970,7 +2968,7 @@
     </row>
     <row r="3">
       <c r="A3" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="24">
         <v>45687.0</v>
@@ -2978,15 +2976,15 @@
     </row>
     <row r="4">
       <c r="A4" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>8</v>
@@ -2994,54 +2992,54 @@
     </row>
     <row r="6">
       <c r="A6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="89" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="90" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="90" t="s">
+      <c r="C8" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="90" t="s">
+      <c r="D8" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="90" t="s">
+      <c r="E8" s="89"/>
+      <c r="F8" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90" t="s">
+      <c r="G8" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="90" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="90" t="s">
-        <v>95</v>
+      <c r="H8" s="89" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10">
         <v>45614.0</v>
       </c>
-      <c r="B9" s="77" t="s">
-        <v>96</v>
+      <c r="B9" s="76" t="s">
+        <v>92</v>
       </c>
       <c r="C9" s="43" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E9" s="43">
         <v>1.0</v>
       </c>
-      <c r="F9" s="91"/>
-      <c r="G9" s="92">
+      <c r="F9" s="90"/>
+      <c r="G9" s="91">
         <f>E9+E10+E11</f>
         <v>6</v>
       </c>
@@ -3051,15 +3049,15 @@
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="43" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D10" s="43" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E10" s="43">
         <v>2.0</v>
       </c>
-      <c r="F10" s="91"/>
+      <c r="F10" s="90"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
     </row>
@@ -3067,15 +3065,15 @@
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="43" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D11" s="43" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E11" s="43">
         <v>3.0</v>
       </c>
-      <c r="F11" s="91"/>
+      <c r="F11" s="90"/>
       <c r="G11" s="16"/>
       <c r="H11" s="15"/>
     </row>
@@ -3083,140 +3081,140 @@
       <c r="A12" s="10">
         <v>45615.0</v>
       </c>
-      <c r="B12" s="93" t="s">
-        <v>103</v>
+      <c r="B12" s="92" t="s">
+        <v>99</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="91"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="91"/>
-      <c r="G12" s="94"/>
+        <v>100</v>
+      </c>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="93"/>
       <c r="H12" s="15"/>
     </row>
     <row r="13">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" s="91"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="94"/>
+        <v>101</v>
+      </c>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="93"/>
       <c r="H13" s="15"/>
     </row>
     <row r="14">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="94"/>
+        <v>102</v>
+      </c>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="93"/>
       <c r="H14" s="15"/>
     </row>
     <row r="15">
       <c r="A15" s="10">
         <v>45616.0</v>
       </c>
-      <c r="B15" s="93" t="s">
-        <v>107</v>
+      <c r="B15" s="92" t="s">
+        <v>103</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="94"/>
+        <v>104</v>
+      </c>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="93"/>
       <c r="H15" s="15"/>
     </row>
     <row r="16">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="94"/>
+        <v>105</v>
+      </c>
+      <c r="D16" s="90"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="93"/>
       <c r="H16" s="15"/>
     </row>
     <row r="17">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="91"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="91"/>
-      <c r="G17" s="94"/>
+        <v>106</v>
+      </c>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="93"/>
       <c r="H17" s="15"/>
     </row>
     <row r="18">
       <c r="A18" s="13">
         <v>45617.0</v>
       </c>
-      <c r="B18" s="91"/>
-      <c r="C18" s="91"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="91"/>
-      <c r="G18" s="94"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="93"/>
       <c r="H18" s="15"/>
     </row>
     <row r="19">
       <c r="A19" s="13">
         <v>45618.0</v>
       </c>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="94"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="93"/>
       <c r="H19" s="15"/>
     </row>
     <row r="20">
       <c r="A20" s="13">
         <v>45621.0</v>
       </c>
-      <c r="B20" s="91"/>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="94"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="93"/>
       <c r="H20" s="15"/>
     </row>
     <row r="21">
       <c r="A21" s="13">
         <v>45622.0</v>
       </c>
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="91"/>
-      <c r="G21" s="94"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="93"/>
       <c r="H21" s="15"/>
     </row>
     <row r="22">
       <c r="A22" s="13">
         <v>45623.0</v>
       </c>
-      <c r="B22" s="91"/>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="94"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="93"/>
       <c r="H22" s="15"/>
     </row>
     <row r="23">
@@ -3224,459 +3222,459 @@
         <v>45624.0</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="C23" s="91"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="94"/>
+        <v>107</v>
+      </c>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="93"/>
       <c r="H23" s="15"/>
     </row>
     <row r="24">
       <c r="A24" s="13">
         <v>45625.0</v>
       </c>
-      <c r="B24" s="91"/>
-      <c r="C24" s="91"/>
-      <c r="D24" s="91"/>
-      <c r="E24" s="91"/>
-      <c r="F24" s="91"/>
-      <c r="G24" s="94"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="93"/>
       <c r="H24" s="15"/>
     </row>
     <row r="25">
       <c r="A25" s="13">
         <v>45628.0</v>
       </c>
-      <c r="B25" s="91"/>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="94"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="93"/>
       <c r="H25" s="15"/>
     </row>
     <row r="26">
       <c r="A26" s="13">
         <v>45629.0</v>
       </c>
-      <c r="B26" s="91"/>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="94"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="93"/>
       <c r="H26" s="15"/>
     </row>
     <row r="27">
       <c r="A27" s="13">
         <v>45630.0</v>
       </c>
-      <c r="B27" s="91"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="91"/>
-      <c r="G27" s="94"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="93"/>
       <c r="H27" s="15"/>
     </row>
     <row r="28">
       <c r="A28" s="13">
         <v>45631.0</v>
       </c>
-      <c r="B28" s="91"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="91"/>
-      <c r="E28" s="91"/>
-      <c r="F28" s="91"/>
-      <c r="G28" s="94"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="93"/>
       <c r="H28" s="15"/>
     </row>
     <row r="29">
       <c r="A29" s="13">
         <v>45635.0</v>
       </c>
-      <c r="B29" s="91"/>
-      <c r="C29" s="91"/>
-      <c r="D29" s="91"/>
-      <c r="E29" s="91"/>
-      <c r="F29" s="91"/>
-      <c r="G29" s="94"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="90"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="93"/>
       <c r="H29" s="15"/>
     </row>
     <row r="30">
       <c r="A30" s="13">
         <v>45636.0</v>
       </c>
-      <c r="B30" s="91"/>
-      <c r="C30" s="91"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="91"/>
-      <c r="F30" s="91"/>
-      <c r="G30" s="94"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="93"/>
       <c r="H30" s="15"/>
     </row>
     <row r="31">
       <c r="A31" s="13">
         <v>45637.0</v>
       </c>
-      <c r="B31" s="91"/>
-      <c r="C31" s="91"/>
-      <c r="D31" s="91"/>
-      <c r="E31" s="91"/>
-      <c r="F31" s="91"/>
-      <c r="G31" s="94"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="90"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="93"/>
       <c r="H31" s="15"/>
     </row>
     <row r="32">
       <c r="A32" s="13">
         <v>45638.0</v>
       </c>
-      <c r="B32" s="91"/>
-      <c r="C32" s="91"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="91"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="94"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
+      <c r="G32" s="93"/>
       <c r="H32" s="15"/>
     </row>
     <row r="33">
       <c r="A33" s="13">
         <v>45639.0</v>
       </c>
-      <c r="B33" s="91"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="94"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="90"/>
+      <c r="D33" s="90"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="93"/>
       <c r="H33" s="15"/>
     </row>
     <row r="34">
       <c r="A34" s="13">
         <v>45642.0</v>
       </c>
-      <c r="B34" s="91"/>
-      <c r="C34" s="91"/>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="94"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="93"/>
       <c r="H34" s="15"/>
     </row>
     <row r="35">
       <c r="A35" s="13">
         <v>45643.0</v>
       </c>
-      <c r="B35" s="91"/>
-      <c r="C35" s="91"/>
-      <c r="D35" s="91"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="91"/>
-      <c r="G35" s="94"/>
+      <c r="B35" s="90"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="93"/>
       <c r="H35" s="15"/>
     </row>
     <row r="36">
       <c r="A36" s="13">
         <v>45644.0</v>
       </c>
-      <c r="B36" s="91"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="91"/>
-      <c r="E36" s="91"/>
-      <c r="F36" s="91"/>
-      <c r="G36" s="94"/>
+      <c r="B36" s="90"/>
+      <c r="C36" s="90"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="90"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="93"/>
       <c r="H36" s="15"/>
     </row>
     <row r="37">
       <c r="A37" s="13">
         <v>45645.0</v>
       </c>
-      <c r="B37" s="91"/>
-      <c r="C37" s="91"/>
-      <c r="D37" s="91"/>
-      <c r="E37" s="91"/>
-      <c r="F37" s="91"/>
-      <c r="G37" s="94"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="90"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="90"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="93"/>
       <c r="H37" s="15"/>
     </row>
     <row r="38">
       <c r="A38" s="13">
         <v>45646.0</v>
       </c>
-      <c r="B38" s="91"/>
-      <c r="C38" s="91"/>
-      <c r="D38" s="91"/>
-      <c r="E38" s="91"/>
-      <c r="F38" s="91"/>
-      <c r="G38" s="94"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="90"/>
+      <c r="D38" s="90"/>
+      <c r="E38" s="90"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="93"/>
       <c r="H38" s="15"/>
     </row>
     <row r="39">
       <c r="A39" s="13">
         <v>45663.0</v>
       </c>
-      <c r="B39" s="91"/>
-      <c r="C39" s="91"/>
-      <c r="D39" s="91"/>
-      <c r="E39" s="91"/>
-      <c r="F39" s="91"/>
-      <c r="G39" s="94"/>
+      <c r="B39" s="90"/>
+      <c r="C39" s="90"/>
+      <c r="D39" s="90"/>
+      <c r="E39" s="90"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="93"/>
       <c r="H39" s="15"/>
     </row>
     <row r="40">
       <c r="A40" s="13">
         <v>45664.0</v>
       </c>
-      <c r="B40" s="91"/>
-      <c r="C40" s="91"/>
-      <c r="D40" s="91"/>
-      <c r="E40" s="91"/>
-      <c r="F40" s="91"/>
-      <c r="G40" s="94"/>
+      <c r="B40" s="90"/>
+      <c r="C40" s="90"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="90"/>
+      <c r="G40" s="93"/>
       <c r="H40" s="15"/>
     </row>
     <row r="41">
       <c r="A41" s="13">
         <v>45665.0</v>
       </c>
-      <c r="B41" s="91"/>
-      <c r="C41" s="91"/>
-      <c r="D41" s="91"/>
-      <c r="E41" s="91"/>
-      <c r="F41" s="91"/>
-      <c r="G41" s="94"/>
+      <c r="B41" s="90"/>
+      <c r="C41" s="90"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="90"/>
+      <c r="G41" s="93"/>
       <c r="H41" s="15"/>
     </row>
     <row r="42">
       <c r="A42" s="13">
         <v>45666.0</v>
       </c>
-      <c r="B42" s="91"/>
-      <c r="C42" s="91"/>
-      <c r="D42" s="91"/>
-      <c r="E42" s="91"/>
-      <c r="F42" s="91"/>
-      <c r="G42" s="94"/>
+      <c r="B42" s="90"/>
+      <c r="C42" s="90"/>
+      <c r="D42" s="90"/>
+      <c r="E42" s="90"/>
+      <c r="F42" s="90"/>
+      <c r="G42" s="93"/>
       <c r="H42" s="15"/>
     </row>
     <row r="43">
       <c r="A43" s="13">
         <v>45667.0</v>
       </c>
-      <c r="B43" s="91"/>
-      <c r="C43" s="91"/>
-      <c r="D43" s="91"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="94"/>
+      <c r="B43" s="90"/>
+      <c r="C43" s="90"/>
+      <c r="D43" s="90"/>
+      <c r="E43" s="90"/>
+      <c r="F43" s="90"/>
+      <c r="G43" s="93"/>
       <c r="H43" s="15"/>
     </row>
     <row r="44">
       <c r="A44" s="13">
         <v>45670.0</v>
       </c>
-      <c r="B44" s="91"/>
-      <c r="C44" s="91"/>
-      <c r="D44" s="91"/>
-      <c r="E44" s="91"/>
-      <c r="F44" s="91"/>
-      <c r="G44" s="94"/>
+      <c r="B44" s="90"/>
+      <c r="C44" s="90"/>
+      <c r="D44" s="90"/>
+      <c r="E44" s="90"/>
+      <c r="F44" s="90"/>
+      <c r="G44" s="93"/>
       <c r="H44" s="15"/>
     </row>
     <row r="45">
       <c r="A45" s="13">
         <v>45671.0</v>
       </c>
-      <c r="B45" s="91"/>
-      <c r="C45" s="91"/>
-      <c r="D45" s="91"/>
-      <c r="E45" s="91"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="94"/>
+      <c r="B45" s="90"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="93"/>
       <c r="H45" s="15"/>
     </row>
     <row r="46">
       <c r="A46" s="13">
         <v>45672.0</v>
       </c>
-      <c r="B46" s="91"/>
-      <c r="C46" s="91"/>
-      <c r="D46" s="91"/>
-      <c r="E46" s="91"/>
-      <c r="F46" s="91"/>
-      <c r="G46" s="94"/>
+      <c r="B46" s="90"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="90"/>
+      <c r="F46" s="90"/>
+      <c r="G46" s="93"/>
       <c r="H46" s="15"/>
     </row>
     <row r="47">
       <c r="A47" s="13">
         <v>45673.0</v>
       </c>
-      <c r="B47" s="91"/>
-      <c r="C47" s="91"/>
-      <c r="D47" s="91"/>
-      <c r="E47" s="91"/>
-      <c r="F47" s="91"/>
-      <c r="G47" s="94"/>
+      <c r="B47" s="90"/>
+      <c r="C47" s="90"/>
+      <c r="D47" s="90"/>
+      <c r="E47" s="90"/>
+      <c r="F47" s="90"/>
+      <c r="G47" s="93"/>
       <c r="H47" s="15"/>
     </row>
     <row r="48">
       <c r="A48" s="13">
         <v>45674.0</v>
       </c>
-      <c r="B48" s="91"/>
-      <c r="C48" s="91"/>
-      <c r="D48" s="91"/>
-      <c r="E48" s="91"/>
-      <c r="F48" s="91"/>
-      <c r="G48" s="94"/>
+      <c r="B48" s="90"/>
+      <c r="C48" s="90"/>
+      <c r="D48" s="90"/>
+      <c r="E48" s="90"/>
+      <c r="F48" s="90"/>
+      <c r="G48" s="93"/>
       <c r="H48" s="15"/>
     </row>
     <row r="49">
       <c r="A49" s="13">
         <v>45677.0</v>
       </c>
-      <c r="B49" s="91"/>
-      <c r="C49" s="91"/>
-      <c r="D49" s="91"/>
-      <c r="E49" s="91"/>
-      <c r="F49" s="91"/>
-      <c r="G49" s="94"/>
+      <c r="B49" s="90"/>
+      <c r="C49" s="90"/>
+      <c r="D49" s="90"/>
+      <c r="E49" s="90"/>
+      <c r="F49" s="90"/>
+      <c r="G49" s="93"/>
       <c r="H49" s="15"/>
     </row>
     <row r="50">
       <c r="A50" s="13">
         <v>45678.0</v>
       </c>
-      <c r="B50" s="91"/>
-      <c r="C50" s="91"/>
-      <c r="D50" s="91"/>
-      <c r="E50" s="91"/>
-      <c r="F50" s="91"/>
-      <c r="G50" s="94"/>
+      <c r="B50" s="90"/>
+      <c r="C50" s="90"/>
+      <c r="D50" s="90"/>
+      <c r="E50" s="90"/>
+      <c r="F50" s="90"/>
+      <c r="G50" s="93"/>
       <c r="H50" s="15"/>
     </row>
     <row r="51">
       <c r="A51" s="13">
         <v>45679.0</v>
       </c>
-      <c r="B51" s="91"/>
-      <c r="C51" s="91"/>
-      <c r="D51" s="91"/>
-      <c r="E51" s="91"/>
-      <c r="F51" s="91"/>
-      <c r="G51" s="94"/>
+      <c r="B51" s="90"/>
+      <c r="C51" s="90"/>
+      <c r="D51" s="90"/>
+      <c r="E51" s="90"/>
+      <c r="F51" s="90"/>
+      <c r="G51" s="93"/>
       <c r="H51" s="15"/>
     </row>
     <row r="52">
       <c r="A52" s="13">
         <v>45680.0</v>
       </c>
-      <c r="B52" s="91"/>
-      <c r="C52" s="91"/>
-      <c r="D52" s="91"/>
-      <c r="E52" s="91"/>
-      <c r="F52" s="91"/>
-      <c r="G52" s="94"/>
+      <c r="B52" s="90"/>
+      <c r="C52" s="90"/>
+      <c r="D52" s="90"/>
+      <c r="E52" s="90"/>
+      <c r="F52" s="90"/>
+      <c r="G52" s="93"/>
       <c r="H52" s="15"/>
     </row>
     <row r="53">
       <c r="A53" s="13">
         <v>45681.0</v>
       </c>
-      <c r="B53" s="91"/>
-      <c r="C53" s="91"/>
-      <c r="D53" s="91"/>
-      <c r="E53" s="91"/>
-      <c r="F53" s="91"/>
-      <c r="G53" s="94"/>
+      <c r="B53" s="90"/>
+      <c r="C53" s="90"/>
+      <c r="D53" s="90"/>
+      <c r="E53" s="90"/>
+      <c r="F53" s="90"/>
+      <c r="G53" s="93"/>
       <c r="H53" s="15"/>
     </row>
     <row r="54">
       <c r="A54" s="13">
         <v>45684.0</v>
       </c>
-      <c r="B54" s="91"/>
-      <c r="C54" s="91"/>
-      <c r="D54" s="91"/>
-      <c r="E54" s="91"/>
-      <c r="F54" s="91"/>
-      <c r="G54" s="94"/>
+      <c r="B54" s="90"/>
+      <c r="C54" s="90"/>
+      <c r="D54" s="90"/>
+      <c r="E54" s="90"/>
+      <c r="F54" s="90"/>
+      <c r="G54" s="93"/>
       <c r="H54" s="15"/>
     </row>
     <row r="55">
       <c r="A55" s="13">
         <v>45685.0</v>
       </c>
-      <c r="B55" s="91"/>
-      <c r="C55" s="91"/>
-      <c r="D55" s="91"/>
-      <c r="E55" s="91"/>
-      <c r="F55" s="91"/>
-      <c r="G55" s="94"/>
+      <c r="B55" s="90"/>
+      <c r="C55" s="90"/>
+      <c r="D55" s="90"/>
+      <c r="E55" s="90"/>
+      <c r="F55" s="90"/>
+      <c r="G55" s="93"/>
       <c r="H55" s="15"/>
     </row>
     <row r="56">
       <c r="A56" s="13">
         <v>45686.0</v>
       </c>
-      <c r="B56" s="91"/>
-      <c r="C56" s="91"/>
-      <c r="D56" s="91"/>
-      <c r="E56" s="91"/>
-      <c r="F56" s="91"/>
-      <c r="G56" s="94"/>
+      <c r="B56" s="90"/>
+      <c r="C56" s="90"/>
+      <c r="D56" s="90"/>
+      <c r="E56" s="90"/>
+      <c r="F56" s="90"/>
+      <c r="G56" s="93"/>
       <c r="H56" s="15"/>
     </row>
     <row r="57">
       <c r="A57" s="13">
         <v>45687.0</v>
       </c>
-      <c r="B57" s="91"/>
-      <c r="C57" s="91"/>
-      <c r="D57" s="91"/>
-      <c r="E57" s="91"/>
-      <c r="F57" s="91"/>
-      <c r="G57" s="94"/>
+      <c r="B57" s="90"/>
+      <c r="C57" s="90"/>
+      <c r="D57" s="90"/>
+      <c r="E57" s="90"/>
+      <c r="F57" s="90"/>
+      <c r="G57" s="93"/>
       <c r="H57" s="16"/>
     </row>
     <row r="58">
       <c r="A58" s="20"/>
-      <c r="G58" s="89"/>
+      <c r="G58" s="88"/>
       <c r="H58" s="33">
         <v>24.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="20"/>
-      <c r="G59" s="89"/>
+      <c r="G59" s="88"/>
     </row>
     <row r="60">
       <c r="A60" s="20"/>
-      <c r="G60" s="89"/>
+      <c r="G60" s="88"/>
     </row>
     <row r="61">
       <c r="A61" s="20"/>
-      <c r="G61" s="89"/>
+      <c r="G61" s="88"/>
     </row>
     <row r="62">
       <c r="A62" s="20"/>
-      <c r="G62" s="89"/>
+      <c r="G62" s="88"/>
     </row>
     <row r="63">
       <c r="A63" s="20"/>
-      <c r="G63" s="89"/>
+      <c r="G63" s="88"/>
     </row>
     <row r="64">
       <c r="A64" s="20"/>
-      <c r="G64" s="89"/>
+      <c r="G64" s="88"/>
     </row>
     <row r="65">
-      <c r="G65" s="89"/>
+      <c r="G65" s="88"/>
     </row>
     <row r="66">
-      <c r="G66" s="89"/>
+      <c r="G66" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3711,740 +3709,643 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="95" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
+      <c r="A1" s="94" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
     </row>
     <row r="2">
-      <c r="A2" s="95" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="97">
+      <c r="A2" s="94" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="96">
         <v>45614.0</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="98" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="D3" s="97" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="99">
+      <c r="A4" s="98">
         <v>45614.0</v>
       </c>
-      <c r="B4" s="100">
+      <c r="B4" s="99">
         <v>0.375</v>
       </c>
-      <c r="C4" s="100">
+      <c r="C4" s="99">
         <v>0.625</v>
       </c>
-      <c r="D4" s="101">
+      <c r="D4" s="100">
         <v>0.25</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="102">
+      <c r="A5" s="101">
         <v>45615.0</v>
       </c>
-      <c r="B5" s="100">
+      <c r="B5" s="99">
         <v>0.375</v>
       </c>
-      <c r="C5" s="100">
+      <c r="C5" s="99">
         <v>0.625</v>
       </c>
-      <c r="D5" s="101">
+      <c r="D5" s="100">
         <v>0.25</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="102">
+      <c r="A6" s="101">
         <v>45616.0</v>
       </c>
-      <c r="B6" s="100">
+      <c r="B6" s="99">
         <v>0.375</v>
       </c>
-      <c r="C6" s="100">
+      <c r="C6" s="99">
         <v>0.625</v>
       </c>
-      <c r="D6" s="101">
+      <c r="D6" s="100">
         <v>0.25</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="102">
+      <c r="A7" s="101">
         <v>45617.0</v>
       </c>
-      <c r="B7" s="100">
+      <c r="B7" s="99">
         <v>0.375</v>
       </c>
-      <c r="C7" s="100">
+      <c r="C7" s="99">
         <v>0.625</v>
       </c>
-      <c r="D7" s="101">
+      <c r="D7" s="100">
         <v>0.25</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="102">
+      <c r="A8" s="101">
         <v>45618.0</v>
       </c>
-      <c r="B8" s="100">
+      <c r="B8" s="99">
         <v>0.375</v>
       </c>
-      <c r="C8" s="100">
+      <c r="C8" s="99">
         <v>0.625</v>
       </c>
-      <c r="D8" s="101">
+      <c r="D8" s="100">
         <v>0.25</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="102">
+      <c r="A9" s="101">
         <v>45621.0</v>
       </c>
-      <c r="B9" s="100">
+      <c r="B9" s="99">
         <v>0.375</v>
       </c>
-      <c r="C9" s="100">
+      <c r="C9" s="99">
         <v>0.625</v>
       </c>
-      <c r="D9" s="101">
+      <c r="D9" s="100">
         <v>0.25</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="102">
+      <c r="A10" s="101">
         <v>45622.0</v>
       </c>
-      <c r="B10" s="103">
+      <c r="B10" s="102">
         <v>0.375</v>
       </c>
-      <c r="C10" s="100">
+      <c r="C10" s="99">
         <v>0.625</v>
       </c>
-      <c r="D10" s="104">
+      <c r="D10" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="102">
+      <c r="A11" s="101">
         <v>45623.0</v>
       </c>
-      <c r="B11" s="103">
+      <c r="B11" s="102">
         <v>0.375</v>
       </c>
-      <c r="C11" s="100">
+      <c r="C11" s="99">
         <v>0.625</v>
       </c>
-      <c r="D11" s="104">
+      <c r="D11" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="102">
+      <c r="A12" s="101">
         <v>45624.0</v>
       </c>
-      <c r="B12" s="103">
+      <c r="B12" s="102">
         <v>0.375</v>
       </c>
-      <c r="C12" s="100">
+      <c r="C12" s="99">
         <v>0.625</v>
       </c>
-      <c r="D12" s="104">
+      <c r="D12" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="102">
+      <c r="A13" s="101">
         <v>45625.0</v>
       </c>
-      <c r="B13" s="103">
+      <c r="B13" s="102">
         <v>0.375</v>
       </c>
-      <c r="C13" s="100">
+      <c r="C13" s="99">
         <v>0.625</v>
       </c>
-      <c r="D13" s="104">
+      <c r="D13" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="102">
+      <c r="A14" s="101">
         <v>45628.0</v>
       </c>
-      <c r="B14" s="103">
+      <c r="B14" s="102">
         <v>0.375</v>
       </c>
-      <c r="C14" s="100">
+      <c r="C14" s="99">
         <v>0.625</v>
       </c>
-      <c r="D14" s="104">
+      <c r="D14" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="102">
+      <c r="A15" s="101">
         <v>45629.0</v>
       </c>
-      <c r="B15" s="103">
+      <c r="B15" s="102">
         <v>0.375</v>
       </c>
-      <c r="C15" s="100">
+      <c r="C15" s="99">
         <v>0.625</v>
       </c>
-      <c r="D15" s="104">
+      <c r="D15" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="102">
+      <c r="A16" s="101">
         <v>45630.0</v>
       </c>
-      <c r="B16" s="103">
+      <c r="B16" s="102">
         <v>0.375</v>
       </c>
-      <c r="C16" s="100">
+      <c r="C16" s="99">
         <v>0.625</v>
       </c>
-      <c r="D16" s="104">
+      <c r="D16" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="102">
+      <c r="A17" s="101">
         <v>45631.0</v>
       </c>
-      <c r="B17" s="103">
+      <c r="B17" s="102">
         <v>0.375</v>
       </c>
-      <c r="C17" s="100">
+      <c r="C17" s="99">
         <v>0.625</v>
       </c>
-      <c r="D17" s="104">
+      <c r="D17" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="102">
-        <v>45632.0</v>
-      </c>
-      <c r="B18" s="103"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="33" t="s">
-        <v>118</v>
+      <c r="A18" s="101">
+        <v>45635.0</v>
+      </c>
+      <c r="B18" s="102">
+        <v>0.375</v>
+      </c>
+      <c r="C18" s="99">
+        <v>0.625</v>
+      </c>
+      <c r="D18" s="103">
+        <v>0.25</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="102">
-        <v>45635.0</v>
-      </c>
-      <c r="B19" s="103">
+      <c r="A19" s="101">
+        <v>45636.0</v>
+      </c>
+      <c r="B19" s="102">
         <v>0.375</v>
       </c>
-      <c r="C19" s="100">
+      <c r="C19" s="99">
         <v>0.625</v>
       </c>
-      <c r="D19" s="104">
+      <c r="D19" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="102">
-        <v>45636.0</v>
-      </c>
-      <c r="B20" s="103">
+      <c r="A20" s="101">
+        <v>45637.0</v>
+      </c>
+      <c r="B20" s="102">
         <v>0.375</v>
       </c>
-      <c r="C20" s="100">
+      <c r="C20" s="99">
         <v>0.625</v>
       </c>
-      <c r="D20" s="104">
+      <c r="D20" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="102">
-        <v>45637.0</v>
-      </c>
-      <c r="B21" s="103">
+      <c r="A21" s="101">
+        <v>45638.0</v>
+      </c>
+      <c r="B21" s="102">
         <v>0.375</v>
       </c>
-      <c r="C21" s="100">
+      <c r="C21" s="99">
         <v>0.625</v>
       </c>
-      <c r="D21" s="104">
+      <c r="D21" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="102">
-        <v>45638.0</v>
-      </c>
-      <c r="B22" s="103">
+      <c r="A22" s="101">
+        <v>45639.0</v>
+      </c>
+      <c r="B22" s="102">
         <v>0.375</v>
       </c>
-      <c r="C22" s="100">
+      <c r="C22" s="99">
         <v>0.625</v>
       </c>
-      <c r="D22" s="104">
+      <c r="D22" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="102">
-        <v>45639.0</v>
-      </c>
-      <c r="B23" s="103">
+      <c r="A23" s="101">
+        <v>45642.0</v>
+      </c>
+      <c r="B23" s="102">
         <v>0.375</v>
       </c>
-      <c r="C23" s="100">
+      <c r="C23" s="99">
         <v>0.625</v>
       </c>
-      <c r="D23" s="104">
+      <c r="D23" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="102">
-        <v>45642.0</v>
-      </c>
-      <c r="B24" s="103">
+      <c r="A24" s="101">
+        <v>45643.0</v>
+      </c>
+      <c r="B24" s="102">
         <v>0.375</v>
       </c>
-      <c r="C24" s="100">
+      <c r="C24" s="99">
         <v>0.625</v>
       </c>
-      <c r="D24" s="104">
+      <c r="D24" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="102">
-        <v>45643.0</v>
-      </c>
-      <c r="B25" s="103">
+      <c r="A25" s="101">
+        <v>45644.0</v>
+      </c>
+      <c r="B25" s="102">
         <v>0.375</v>
       </c>
-      <c r="C25" s="100">
+      <c r="C25" s="99">
         <v>0.625</v>
       </c>
-      <c r="D25" s="104">
+      <c r="D25" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="102">
-        <v>45644.0</v>
-      </c>
-      <c r="B26" s="103">
+      <c r="A26" s="101">
+        <v>45645.0</v>
+      </c>
+      <c r="B26" s="102">
         <v>0.375</v>
       </c>
-      <c r="C26" s="100">
+      <c r="C26" s="99">
         <v>0.625</v>
       </c>
-      <c r="D26" s="104">
+      <c r="D26" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="102">
-        <v>45645.0</v>
-      </c>
-      <c r="B27" s="103">
+      <c r="A27" s="101">
+        <v>45646.0</v>
+      </c>
+      <c r="B27" s="102">
         <v>0.375</v>
       </c>
-      <c r="C27" s="100">
+      <c r="C27" s="99">
         <v>0.625</v>
       </c>
-      <c r="D27" s="104">
+      <c r="D27" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="102">
-        <v>45646.0</v>
-      </c>
-      <c r="B28" s="103">
+      <c r="A28" s="101">
+        <v>45663.0</v>
+      </c>
+      <c r="B28" s="102">
         <v>0.375</v>
       </c>
-      <c r="C28" s="100">
+      <c r="C28" s="99">
         <v>0.625</v>
       </c>
-      <c r="D28" s="104">
+      <c r="D28" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="102">
-        <v>45649.0</v>
-      </c>
-      <c r="B29" s="103"/>
-      <c r="C29" s="103"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="105" t="s">
-        <v>119</v>
+      <c r="A29" s="101">
+        <v>45664.0</v>
+      </c>
+      <c r="B29" s="102">
+        <v>0.375</v>
+      </c>
+      <c r="C29" s="99">
+        <v>0.625</v>
+      </c>
+      <c r="D29" s="103">
+        <v>0.25</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="102">
-        <v>45650.0</v>
-      </c>
-      <c r="B30" s="103"/>
-      <c r="C30" s="103"/>
-      <c r="D30" s="104"/>
+      <c r="A30" s="101">
+        <v>45665.0</v>
+      </c>
+      <c r="B30" s="102">
+        <v>0.375</v>
+      </c>
+      <c r="C30" s="99">
+        <v>0.625</v>
+      </c>
+      <c r="D30" s="103">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="102">
-        <v>45651.0</v>
-      </c>
-      <c r="B31" s="103"/>
-      <c r="C31" s="103"/>
-      <c r="D31" s="104"/>
+      <c r="A31" s="101">
+        <v>45666.0</v>
+      </c>
+      <c r="B31" s="102">
+        <v>0.375</v>
+      </c>
+      <c r="C31" s="99">
+        <v>0.625</v>
+      </c>
+      <c r="D31" s="103">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="102">
-        <v>45652.0</v>
-      </c>
-      <c r="B32" s="103"/>
-      <c r="C32" s="103"/>
-      <c r="D32" s="104"/>
+      <c r="A32" s="101">
+        <v>45667.0</v>
+      </c>
+      <c r="B32" s="99">
+        <v>0.375</v>
+      </c>
+      <c r="C32" s="99">
+        <v>0.625</v>
+      </c>
+      <c r="D32" s="100">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="102">
-        <v>45653.0</v>
-      </c>
-      <c r="B33" s="103"/>
-      <c r="C33" s="103"/>
-      <c r="D33" s="104"/>
+      <c r="A33" s="101">
+        <v>45670.0</v>
+      </c>
+      <c r="B33" s="102">
+        <v>0.375</v>
+      </c>
+      <c r="C33" s="99">
+        <v>0.625</v>
+      </c>
+      <c r="D33" s="103">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="102">
-        <v>45656.0</v>
-      </c>
-      <c r="B34" s="103"/>
-      <c r="C34" s="103"/>
-      <c r="D34" s="104"/>
+      <c r="A34" s="101">
+        <v>45671.0</v>
+      </c>
+      <c r="B34" s="102">
+        <v>0.375</v>
+      </c>
+      <c r="C34" s="99">
+        <v>0.625</v>
+      </c>
+      <c r="D34" s="103">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="102">
-        <v>45657.0</v>
-      </c>
-      <c r="B35" s="103"/>
-      <c r="C35" s="103"/>
-      <c r="D35" s="104"/>
+      <c r="A35" s="101">
+        <v>45672.0</v>
+      </c>
+      <c r="B35" s="99">
+        <v>0.375</v>
+      </c>
+      <c r="C35" s="99">
+        <v>0.625</v>
+      </c>
+      <c r="D35" s="100">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="102">
-        <v>45658.0</v>
-      </c>
-      <c r="B36" s="103"/>
-      <c r="C36" s="103"/>
-      <c r="D36" s="104"/>
+      <c r="A36" s="101">
+        <v>45673.0</v>
+      </c>
+      <c r="B36" s="99">
+        <v>0.375</v>
+      </c>
+      <c r="C36" s="99">
+        <v>0.625</v>
+      </c>
+      <c r="D36" s="100">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="102">
-        <v>45659.0</v>
-      </c>
-      <c r="B37" s="103"/>
-      <c r="C37" s="103"/>
-      <c r="D37" s="104"/>
+      <c r="A37" s="101">
+        <v>45674.0</v>
+      </c>
+      <c r="B37" s="102">
+        <v>0.375</v>
+      </c>
+      <c r="C37" s="99">
+        <v>0.625</v>
+      </c>
+      <c r="D37" s="103">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="102">
-        <v>45660.0</v>
-      </c>
-      <c r="B38" s="103"/>
-      <c r="C38" s="103"/>
-      <c r="D38" s="104"/>
+      <c r="A38" s="101">
+        <v>45677.0</v>
+      </c>
+      <c r="B38" s="99">
+        <v>0.375</v>
+      </c>
+      <c r="C38" s="99">
+        <v>0.625</v>
+      </c>
+      <c r="D38" s="100">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="102">
-        <v>45663.0</v>
-      </c>
-      <c r="B39" s="103">
+      <c r="A39" s="101">
+        <v>45678.0</v>
+      </c>
+      <c r="B39" s="99">
         <v>0.375</v>
       </c>
-      <c r="C39" s="100">
+      <c r="C39" s="99">
         <v>0.625</v>
       </c>
-      <c r="D39" s="104">
+      <c r="D39" s="100">
         <v>0.25</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="102">
-        <v>45664.0</v>
-      </c>
-      <c r="B40" s="103">
+      <c r="A40" s="101">
+        <v>45679.0</v>
+      </c>
+      <c r="B40" s="102">
         <v>0.375</v>
       </c>
-      <c r="C40" s="100">
+      <c r="C40" s="99">
         <v>0.625</v>
       </c>
-      <c r="D40" s="104">
+      <c r="D40" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="102">
-        <v>45665.0</v>
-      </c>
-      <c r="B41" s="103">
+      <c r="A41" s="101">
+        <v>45680.0</v>
+      </c>
+      <c r="B41" s="102">
         <v>0.375</v>
       </c>
-      <c r="C41" s="100">
+      <c r="C41" s="99">
         <v>0.625</v>
       </c>
-      <c r="D41" s="104">
+      <c r="D41" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="102">
-        <v>45666.0</v>
-      </c>
-      <c r="B42" s="103">
+      <c r="A42" s="101">
+        <v>45681.0</v>
+      </c>
+      <c r="B42" s="102">
         <v>0.375</v>
       </c>
-      <c r="C42" s="100">
+      <c r="C42" s="99">
         <v>0.625</v>
       </c>
-      <c r="D42" s="104">
+      <c r="D42" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="102">
-        <v>45667.0</v>
-      </c>
-      <c r="B43" s="100">
+      <c r="A43" s="101">
+        <v>45684.0</v>
+      </c>
+      <c r="B43" s="99">
         <v>0.375</v>
       </c>
-      <c r="C43" s="100">
+      <c r="C43" s="99">
         <v>0.625</v>
       </c>
-      <c r="D43" s="101">
+      <c r="D43" s="100">
         <v>0.25</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="102">
-        <v>45670.0</v>
-      </c>
-      <c r="B44" s="103">
+      <c r="A44" s="101">
+        <v>45685.0</v>
+      </c>
+      <c r="B44" s="102">
         <v>0.375</v>
       </c>
-      <c r="C44" s="100">
+      <c r="C44" s="99">
         <v>0.625</v>
       </c>
-      <c r="D44" s="104">
+      <c r="D44" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="102">
-        <v>45671.0</v>
-      </c>
-      <c r="B45" s="103">
+      <c r="A45" s="101">
+        <v>45686.0</v>
+      </c>
+      <c r="B45" s="102">
         <v>0.375</v>
       </c>
-      <c r="C45" s="100">
+      <c r="C45" s="99">
         <v>0.625</v>
       </c>
-      <c r="D45" s="104">
+      <c r="D45" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="102">
-        <v>45672.0</v>
-      </c>
-      <c r="B46" s="100">
+      <c r="A46" s="101">
+        <v>45687.0</v>
+      </c>
+      <c r="B46" s="102">
         <v>0.375</v>
       </c>
-      <c r="C46" s="100">
+      <c r="C46" s="99">
         <v>0.625</v>
       </c>
-      <c r="D46" s="101">
+      <c r="D46" s="103">
         <v>0.25</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="102">
-        <v>45673.0</v>
-      </c>
-      <c r="B47" s="100">
-        <v>0.375</v>
-      </c>
-      <c r="C47" s="100">
-        <v>0.625</v>
-      </c>
-      <c r="D47" s="101">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="102">
-        <v>45674.0</v>
-      </c>
-      <c r="B48" s="103">
-        <v>0.375</v>
-      </c>
-      <c r="C48" s="100">
-        <v>0.625</v>
-      </c>
-      <c r="D48" s="104">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="102">
-        <v>45677.0</v>
-      </c>
-      <c r="B49" s="100">
-        <v>0.375</v>
-      </c>
-      <c r="C49" s="100">
-        <v>0.625</v>
-      </c>
-      <c r="D49" s="101">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="102">
-        <v>45678.0</v>
-      </c>
-      <c r="B50" s="100">
-        <v>0.375</v>
-      </c>
-      <c r="C50" s="100">
-        <v>0.625</v>
-      </c>
-      <c r="D50" s="101">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="102">
-        <v>45679.0</v>
-      </c>
-      <c r="B51" s="103">
-        <v>0.375</v>
-      </c>
-      <c r="C51" s="100">
-        <v>0.625</v>
-      </c>
-      <c r="D51" s="104">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="102">
-        <v>45680.0</v>
-      </c>
-      <c r="B52" s="103">
-        <v>0.375</v>
-      </c>
-      <c r="C52" s="100">
-        <v>0.625</v>
-      </c>
-      <c r="D52" s="104">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="102">
-        <v>45681.0</v>
-      </c>
-      <c r="B53" s="103">
-        <v>0.375</v>
-      </c>
-      <c r="C53" s="100">
-        <v>0.625</v>
-      </c>
-      <c r="D53" s="104">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="102">
-        <v>45684.0</v>
-      </c>
-      <c r="B54" s="100">
-        <v>0.375</v>
-      </c>
-      <c r="C54" s="100">
-        <v>0.625</v>
-      </c>
-      <c r="D54" s="101">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="102">
-        <v>45685.0</v>
-      </c>
-      <c r="B55" s="103">
-        <v>0.375</v>
-      </c>
-      <c r="C55" s="100">
-        <v>0.625</v>
-      </c>
-      <c r="D55" s="104">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="102">
-        <v>45686.0</v>
-      </c>
-      <c r="B56" s="103">
-        <v>0.375</v>
-      </c>
-      <c r="C56" s="100">
-        <v>0.625</v>
-      </c>
-      <c r="D56" s="104">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="102">
-        <v>45687.0</v>
-      </c>
-      <c r="B57" s="103">
-        <v>0.375</v>
-      </c>
-      <c r="C57" s="100">
-        <v>0.625</v>
-      </c>
-      <c r="D57" s="104">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="C58" s="100"/>
+      <c r="C47" s="99"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E29:E38"/>
-  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>